<commit_message>
Update quan ly co dong
</commit_message>
<xml_diff>
--- a/public/files/SchemaCoDong.xlsx
+++ b/public/files/SchemaCoDong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/vote_cms/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BC413B-3456-2443-B144-7F03D5CCED6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950E0664-114E-544C-A286-11424175D95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Mã cổ đông</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Trạng thái BQ</t>
-  </si>
-  <si>
-    <t>Hoạt động</t>
   </si>
 </sst>
 </file>
@@ -429,15 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,9 +464,6 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>